<commit_message>
Added edges for edges and vertices
</commit_message>
<xml_diff>
--- a/BoardList.xlsx
+++ b/BoardList.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MichaelDunn/Desktop/repos/CatanUtility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C22C94E-B232-C14B-ABE2-C54BA40C292D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE16F17A-8456-0D40-A371-241B71BFCB86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{E36BCCCE-4262-5440-9D49-E3EE028E3368}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="13800" windowHeight="17540" activeTab="2" xr2:uid="{E36BCCCE-4262-5440-9D49-E3EE028E3368}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="HexVertices" sheetId="3" r:id="rId3"/>
+    <sheet name="HexEdges" sheetId="4" r:id="rId4"/>
+    <sheet name="EdgeEdges" sheetId="5" r:id="rId5"/>
+    <sheet name="HexEdges1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Edges</t>
   </si>
@@ -68,6 +71,9 @@
   </si>
   <si>
     <t>6th</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -1467,7 +1473,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1518,7 +1524,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B12" si="0">B3+A3</f>
@@ -1537,8 +1543,8 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <f>B4+A4</f>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -1550,11 +1556,11 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -1570,7 +1576,7 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -1582,11 +1588,11 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1602,7 +1608,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -1614,11 +1620,11 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -1634,7 +1640,7 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D11">
         <v>4</v>
@@ -1650,7 +1656,7 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -1663,7 +1669,10 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <f>SUM(A2:A12)</f>
-        <v>64</v>
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -1677,6 +1686,9 @@
       <c r="D14">
         <f>SUM(D2:D13)</f>
         <v>54</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1725,7 +1737,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C20" si="0">(A3*2)-(A3-D3)</f>
+        <f t="shared" ref="C3:C19" si="0">(A3*2)-(A3-D3)</f>
         <v>2</v>
       </c>
       <c r="D3">
@@ -1997,8 +2009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C1BE97-1B95-3B46-89E1-A426DF1BDA1A}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2031,22 +2043,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2078,22 +2090,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2125,22 +2137,22 @@
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -2172,22 +2184,22 @@
         <v>4</v>
       </c>
       <c r="B8" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2219,22 +2231,22 @@
         <v>5</v>
       </c>
       <c r="B10" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -2266,22 +2278,22 @@
         <v>6</v>
       </c>
       <c r="B12" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G12" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -2313,22 +2325,22 @@
         <v>7</v>
       </c>
       <c r="B14" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G14" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -2360,22 +2372,22 @@
         <v>8</v>
       </c>
       <c r="B16" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="3">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="3">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" s="3">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G16" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2407,22 +2419,22 @@
         <v>9</v>
       </c>
       <c r="B18" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="3">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E18" s="3">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F18" s="3">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G18" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -2454,22 +2466,22 @@
         <v>10</v>
       </c>
       <c r="B20" s="3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="3">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="3">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E20" s="3">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F20" s="3">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G20" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -2501,22 +2513,22 @@
         <v>11</v>
       </c>
       <c r="B22" s="3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="3">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22" s="3">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E22" s="3">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F22" s="3">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G22" s="3">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -2548,22 +2560,22 @@
         <v>12</v>
       </c>
       <c r="B24" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C24" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D24" s="3">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" s="3">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F24" s="3">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G24" s="3">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -2575,19 +2587,19 @@
       </c>
       <c r="D25" s="3">
         <f t="shared" ref="D25:G25" si="11">D24-$B24</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E25" s="3">
         <f t="shared" si="11"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="11"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G25" s="3">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -2595,22 +2607,22 @@
         <v>13</v>
       </c>
       <c r="B26" s="4">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C26" s="4">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" s="4">
+        <v>39</v>
+      </c>
+      <c r="E26" s="4">
+        <v>43</v>
+      </c>
+      <c r="F26" s="4">
         <v>40</v>
       </c>
-      <c r="E26" s="4">
-        <v>44</v>
-      </c>
-      <c r="F26" s="4">
-        <v>39</v>
-      </c>
       <c r="G26" s="4">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -2618,15 +2630,15 @@
       <c r="B27" s="4"/>
       <c r="C27" s="4">
         <f>C26-$B26</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D27" s="4">
         <f t="shared" ref="D27:G27" si="12">D26-$B26</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E27" s="4">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F27" s="4">
         <f t="shared" si="12"/>
@@ -2634,7 +2646,7 @@
       </c>
       <c r="G27" s="4">
         <f t="shared" si="12"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -2642,22 +2654,22 @@
         <v>14</v>
       </c>
       <c r="B28" s="4">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="4">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D28" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E28" s="4">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F28" s="4">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G28" s="4">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -2689,22 +2701,22 @@
         <v>15</v>
       </c>
       <c r="B30" s="4">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="4">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D30" s="4">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E30" s="4">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F30" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G30" s="4">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -2736,22 +2748,22 @@
         <v>16</v>
       </c>
       <c r="B32" s="4">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="4">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D32" s="4">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E32" s="4">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F32" s="4">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G32" s="4">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -2783,22 +2795,22 @@
         <v>17</v>
       </c>
       <c r="B34" s="5">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34" s="5">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D34" s="5">
+        <v>48</v>
+      </c>
+      <c r="E34" s="5">
+        <v>51</v>
+      </c>
+      <c r="F34" s="5">
         <v>49</v>
       </c>
-      <c r="E34" s="5">
-        <v>52</v>
-      </c>
-      <c r="F34" s="5">
-        <v>48</v>
-      </c>
       <c r="G34" s="5">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -2818,7 +2830,7 @@
       </c>
       <c r="F35" s="5">
         <f t="shared" si="16"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G35" s="5">
         <f t="shared" si="16"/>
@@ -2830,22 +2842,22 @@
         <v>18</v>
       </c>
       <c r="B36" s="5">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C36" s="5">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D36" s="5">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E36" s="5">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F36" s="5">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G36" s="5">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -2877,22 +2889,22 @@
         <v>19</v>
       </c>
       <c r="B38" s="5">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" s="5">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D38" s="5">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E38" s="5">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F38" s="5">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G38" s="5">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -2924,4 +2936,2783 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C202B04-E54C-0442-8CDD-7E8BD12EF14B}">
+  <dimension ref="A1:G39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1">
+        <f>C2-$B2</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:G3" si="0">D2-$B2</f>
+        <v>7</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1">
+        <f>C4-$B4</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" ref="D5:G5" si="1">D4-$B4</f>
+        <v>6</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1">
+        <v>15</v>
+      </c>
+      <c r="G6" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1">
+        <f>C6-$B6</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" ref="D7:G7" si="2">D6-$B6</f>
+        <v>5</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2">
+        <v>19</v>
+      </c>
+      <c r="E8" s="2">
+        <v>25</v>
+      </c>
+      <c r="F8" s="2">
+        <v>24</v>
+      </c>
+      <c r="G8" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2">
+        <f>C8-$B8</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" ref="D9:G9" si="3">D8-$B8</f>
+        <v>9</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2">
+        <v>20</v>
+      </c>
+      <c r="E10" s="2">
+        <v>27</v>
+      </c>
+      <c r="F10" s="2">
+        <v>26</v>
+      </c>
+      <c r="G10" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2">
+        <f>C10-$B10</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" ref="D11:G11" si="4">D10-$B10</f>
+        <v>8</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2">
+        <v>21</v>
+      </c>
+      <c r="E12" s="2">
+        <v>29</v>
+      </c>
+      <c r="F12" s="2">
+        <v>28</v>
+      </c>
+      <c r="G12" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2">
+        <f>C12-$B12</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" ref="D13:G13" si="5">D12-$B12</f>
+        <v>7</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2">
+        <v>16</v>
+      </c>
+      <c r="C14" s="2">
+        <v>17</v>
+      </c>
+      <c r="D14" s="2">
+        <v>22</v>
+      </c>
+      <c r="E14" s="2">
+        <v>31</v>
+      </c>
+      <c r="F14" s="2">
+        <v>30</v>
+      </c>
+      <c r="G14" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2">
+        <f>C14-$B14</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" ref="D15:G15" si="6">D14-$B14</f>
+        <v>6</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>8</v>
+      </c>
+      <c r="B16" s="3">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3">
+        <v>24</v>
+      </c>
+      <c r="D16" s="3">
+        <v>34</v>
+      </c>
+      <c r="E16" s="3">
+        <v>40</v>
+      </c>
+      <c r="F16" s="3">
+        <v>39</v>
+      </c>
+      <c r="G16" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3">
+        <f>C16-$B16</f>
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" ref="D17:G17" si="7">D16-$B16</f>
+        <v>11</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="7"/>
+        <v>17</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="G17" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>9</v>
+      </c>
+      <c r="B18" s="3">
+        <v>25</v>
+      </c>
+      <c r="C18" s="3">
+        <v>26</v>
+      </c>
+      <c r="D18" s="3">
+        <v>35</v>
+      </c>
+      <c r="E18" s="3">
+        <v>42</v>
+      </c>
+      <c r="F18" s="3">
+        <v>41</v>
+      </c>
+      <c r="G18" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3">
+        <f>C18-$B18</f>
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" ref="D19:G19" si="8">D18-$B18</f>
+        <v>10</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="8"/>
+        <v>17</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>10</v>
+      </c>
+      <c r="B20" s="3">
+        <v>27</v>
+      </c>
+      <c r="C20" s="3">
+        <v>28</v>
+      </c>
+      <c r="D20" s="3">
+        <v>36</v>
+      </c>
+      <c r="E20" s="3">
+        <v>44</v>
+      </c>
+      <c r="F20" s="3">
+        <v>43</v>
+      </c>
+      <c r="G20" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3">
+        <f>C20-$B20</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" ref="D21:G21" si="9">D20-$B20</f>
+        <v>9</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="9"/>
+        <v>17</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>11</v>
+      </c>
+      <c r="B22" s="3">
+        <v>29</v>
+      </c>
+      <c r="C22" s="3">
+        <v>30</v>
+      </c>
+      <c r="D22" s="3">
+        <v>37</v>
+      </c>
+      <c r="E22" s="3">
+        <v>46</v>
+      </c>
+      <c r="F22" s="3">
+        <v>45</v>
+      </c>
+      <c r="G22" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3">
+        <f>C22-$B22</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" ref="D23:G23" si="10">D22-$B22</f>
+        <v>8</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="10"/>
+        <v>17</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
+      <c r="G23" s="3">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>12</v>
+      </c>
+      <c r="B24" s="3">
+        <v>31</v>
+      </c>
+      <c r="C24" s="3">
+        <v>32</v>
+      </c>
+      <c r="D24" s="3">
+        <v>38</v>
+      </c>
+      <c r="E24" s="3">
+        <v>48</v>
+      </c>
+      <c r="F24" s="3">
+        <v>47</v>
+      </c>
+      <c r="G24" s="3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3">
+        <f>C24-$B24</f>
+        <v>1</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" ref="D25:G25" si="11">D24-$B24</f>
+        <v>7</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="11"/>
+        <v>17</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="11"/>
+        <v>16</v>
+      </c>
+      <c r="G25" s="3">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>13</v>
+      </c>
+      <c r="B26" s="4">
+        <v>40</v>
+      </c>
+      <c r="C26" s="4">
+        <v>41</v>
+      </c>
+      <c r="D26" s="4">
+        <v>50</v>
+      </c>
+      <c r="E26" s="4">
+        <v>55</v>
+      </c>
+      <c r="F26" s="4">
+        <v>54</v>
+      </c>
+      <c r="G26" s="4">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4">
+        <f>C26-$B26</f>
+        <v>1</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" ref="D27:G27" si="12">D26-$B26</f>
+        <v>10</v>
+      </c>
+      <c r="E27" s="4">
+        <f t="shared" si="12"/>
+        <v>15</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" si="12"/>
+        <v>14</v>
+      </c>
+      <c r="G27" s="4">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>14</v>
+      </c>
+      <c r="B28" s="4">
+        <v>42</v>
+      </c>
+      <c r="C28" s="4">
+        <v>43</v>
+      </c>
+      <c r="D28" s="4">
+        <v>51</v>
+      </c>
+      <c r="E28" s="4">
+        <v>57</v>
+      </c>
+      <c r="F28" s="4">
+        <v>56</v>
+      </c>
+      <c r="G28" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4">
+        <f>C28-$B28</f>
+        <v>1</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" ref="D29:G29" si="13">D28-$B28</f>
+        <v>9</v>
+      </c>
+      <c r="E29" s="4">
+        <f t="shared" si="13"/>
+        <v>15</v>
+      </c>
+      <c r="F29" s="4">
+        <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
+      <c r="G29" s="4">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>15</v>
+      </c>
+      <c r="B30" s="4">
+        <v>44</v>
+      </c>
+      <c r="C30" s="4">
+        <v>45</v>
+      </c>
+      <c r="D30" s="4">
+        <v>52</v>
+      </c>
+      <c r="E30" s="4">
+        <v>59</v>
+      </c>
+      <c r="F30" s="4">
+        <v>58</v>
+      </c>
+      <c r="G30" s="4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4">
+        <f>C30-$B30</f>
+        <v>1</v>
+      </c>
+      <c r="D31" s="4">
+        <f t="shared" ref="D31:G31" si="14">D30-$B30</f>
+        <v>8</v>
+      </c>
+      <c r="E31" s="4">
+        <f t="shared" si="14"/>
+        <v>15</v>
+      </c>
+      <c r="F31" s="4">
+        <f t="shared" si="14"/>
+        <v>14</v>
+      </c>
+      <c r="G31" s="4">
+        <f t="shared" si="14"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
+        <v>16</v>
+      </c>
+      <c r="B32" s="4">
+        <v>46</v>
+      </c>
+      <c r="C32" s="4">
+        <v>47</v>
+      </c>
+      <c r="D32" s="4">
+        <v>53</v>
+      </c>
+      <c r="E32" s="4">
+        <v>61</v>
+      </c>
+      <c r="F32" s="4">
+        <v>60</v>
+      </c>
+      <c r="G32" s="4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4">
+        <f>C32-$B32</f>
+        <v>1</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" ref="D33:G33" si="15">D32-$B32</f>
+        <v>7</v>
+      </c>
+      <c r="E33" s="4">
+        <f t="shared" si="15"/>
+        <v>15</v>
+      </c>
+      <c r="F33" s="4">
+        <f t="shared" si="15"/>
+        <v>14</v>
+      </c>
+      <c r="G33" s="4">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>17</v>
+      </c>
+      <c r="B34" s="5">
+        <v>55</v>
+      </c>
+      <c r="C34" s="5">
+        <v>56</v>
+      </c>
+      <c r="D34" s="5">
+        <v>63</v>
+      </c>
+      <c r="E34" s="5">
+        <v>67</v>
+      </c>
+      <c r="F34" s="5">
+        <v>66</v>
+      </c>
+      <c r="G34" s="5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5">
+        <f>C34-$B34</f>
+        <v>1</v>
+      </c>
+      <c r="D35" s="5">
+        <f t="shared" ref="D35:G35" si="16">D34-$B34</f>
+        <v>8</v>
+      </c>
+      <c r="E35" s="5">
+        <f t="shared" si="16"/>
+        <v>12</v>
+      </c>
+      <c r="F35" s="5">
+        <f t="shared" si="16"/>
+        <v>11</v>
+      </c>
+      <c r="G35" s="5">
+        <f t="shared" si="16"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
+        <v>18</v>
+      </c>
+      <c r="B36" s="5">
+        <v>57</v>
+      </c>
+      <c r="C36" s="5">
+        <v>58</v>
+      </c>
+      <c r="D36" s="5">
+        <v>64</v>
+      </c>
+      <c r="E36" s="5">
+        <v>69</v>
+      </c>
+      <c r="F36" s="5">
+        <v>68</v>
+      </c>
+      <c r="G36" s="5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5">
+        <f>C36-$B36</f>
+        <v>1</v>
+      </c>
+      <c r="D37" s="5">
+        <f t="shared" ref="D37:G37" si="17">D36-$B36</f>
+        <v>7</v>
+      </c>
+      <c r="E37" s="5">
+        <f t="shared" si="17"/>
+        <v>12</v>
+      </c>
+      <c r="F37" s="5">
+        <f t="shared" si="17"/>
+        <v>11</v>
+      </c>
+      <c r="G37" s="5">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
+        <v>19</v>
+      </c>
+      <c r="B38" s="5">
+        <v>59</v>
+      </c>
+      <c r="C38" s="5">
+        <v>60</v>
+      </c>
+      <c r="D38" s="5">
+        <v>65</v>
+      </c>
+      <c r="E38" s="5">
+        <v>71</v>
+      </c>
+      <c r="F38" s="5">
+        <v>70</v>
+      </c>
+      <c r="G38" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5">
+        <f>C38-$B38</f>
+        <v>1</v>
+      </c>
+      <c r="D39" s="5">
+        <f t="shared" ref="D39:G39" si="18">D38-$B38</f>
+        <v>6</v>
+      </c>
+      <c r="E39" s="5">
+        <f t="shared" si="18"/>
+        <v>12</v>
+      </c>
+      <c r="F39" s="5">
+        <f t="shared" si="18"/>
+        <v>11</v>
+      </c>
+      <c r="G39" s="5">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D9AFF69-65F7-0740-B4C7-4AD1590C0D8F}">
+  <dimension ref="A1:E72"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>13</v>
+      </c>
+      <c r="E13">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>17</v>
+      </c>
+      <c r="E17">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>23</v>
+      </c>
+      <c r="D19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>11</v>
+      </c>
+      <c r="C20">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>25</v>
+      </c>
+      <c r="E20">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <v>14</v>
+      </c>
+      <c r="D21">
+        <v>27</v>
+      </c>
+      <c r="E21">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>16</v>
+      </c>
+      <c r="D22">
+        <v>29</v>
+      </c>
+      <c r="E22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>17</v>
+      </c>
+      <c r="C23">
+        <v>31</v>
+      </c>
+      <c r="D23">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>18</v>
+      </c>
+      <c r="C24">
+        <v>24</v>
+      </c>
+      <c r="D24">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <v>25</v>
+      </c>
+      <c r="E25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>19</v>
+      </c>
+      <c r="C26">
+        <v>24</v>
+      </c>
+      <c r="D26">
+        <v>26</v>
+      </c>
+      <c r="E26">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>19</v>
+      </c>
+      <c r="C27">
+        <v>25</v>
+      </c>
+      <c r="D27">
+        <v>27</v>
+      </c>
+      <c r="E27">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>26</v>
+      </c>
+      <c r="D28">
+        <v>28</v>
+      </c>
+      <c r="E28">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>27</v>
+      </c>
+      <c r="D29">
+        <v>29</v>
+      </c>
+      <c r="E29">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>21</v>
+      </c>
+      <c r="C30">
+        <v>28</v>
+      </c>
+      <c r="D30">
+        <v>30</v>
+      </c>
+      <c r="E30">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>21</v>
+      </c>
+      <c r="C31">
+        <v>29</v>
+      </c>
+      <c r="D31">
+        <v>21</v>
+      </c>
+      <c r="E31">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>22</v>
+      </c>
+      <c r="C32">
+        <v>30</v>
+      </c>
+      <c r="D32">
+        <v>32</v>
+      </c>
+      <c r="E32">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>22</v>
+      </c>
+      <c r="C33">
+        <v>31</v>
+      </c>
+      <c r="D33">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>23</v>
+      </c>
+      <c r="C34">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>24</v>
+      </c>
+      <c r="C35">
+        <v>25</v>
+      </c>
+      <c r="D35">
+        <v>40</v>
+      </c>
+      <c r="E35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>26</v>
+      </c>
+      <c r="C36">
+        <v>27</v>
+      </c>
+      <c r="D36">
+        <v>42</v>
+      </c>
+      <c r="E36">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>28</v>
+      </c>
+      <c r="C37">
+        <v>29</v>
+      </c>
+      <c r="D37">
+        <v>44</v>
+      </c>
+      <c r="E37">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>30</v>
+      </c>
+      <c r="C38">
+        <v>31</v>
+      </c>
+      <c r="D38">
+        <v>46</v>
+      </c>
+      <c r="E38">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>32</v>
+      </c>
+      <c r="C39">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>33</v>
+      </c>
+      <c r="C40">
+        <v>40</v>
+      </c>
+      <c r="D40">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>34</v>
+      </c>
+      <c r="C41">
+        <v>39</v>
+      </c>
+      <c r="D41">
+        <v>41</v>
+      </c>
+      <c r="E41">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>34</v>
+      </c>
+      <c r="C42">
+        <v>40</v>
+      </c>
+      <c r="D42">
+        <v>42</v>
+      </c>
+      <c r="E42">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>35</v>
+      </c>
+      <c r="C43">
+        <v>41</v>
+      </c>
+      <c r="D43">
+        <v>43</v>
+      </c>
+      <c r="E43">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>35</v>
+      </c>
+      <c r="C44">
+        <v>42</v>
+      </c>
+      <c r="D44">
+        <v>44</v>
+      </c>
+      <c r="E44">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>36</v>
+      </c>
+      <c r="C45">
+        <v>43</v>
+      </c>
+      <c r="D45">
+        <v>45</v>
+      </c>
+      <c r="E45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>36</v>
+      </c>
+      <c r="C46">
+        <v>44</v>
+      </c>
+      <c r="D46">
+        <v>46</v>
+      </c>
+      <c r="E46">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>37</v>
+      </c>
+      <c r="C47">
+        <v>45</v>
+      </c>
+      <c r="D47">
+        <v>47</v>
+      </c>
+      <c r="E47">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>37</v>
+      </c>
+      <c r="C48">
+        <v>46</v>
+      </c>
+      <c r="D48">
+        <v>48</v>
+      </c>
+      <c r="E48">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>38</v>
+      </c>
+      <c r="C49">
+        <v>47</v>
+      </c>
+      <c r="D49">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>39</v>
+      </c>
+      <c r="C50">
+        <v>40</v>
+      </c>
+      <c r="D50">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>41</v>
+      </c>
+      <c r="C51">
+        <v>42</v>
+      </c>
+      <c r="D51">
+        <v>55</v>
+      </c>
+      <c r="E51">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>43</v>
+      </c>
+      <c r="C52">
+        <v>44</v>
+      </c>
+      <c r="D52">
+        <v>57</v>
+      </c>
+      <c r="E52">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>45</v>
+      </c>
+      <c r="C53">
+        <v>46</v>
+      </c>
+      <c r="D53">
+        <v>59</v>
+      </c>
+      <c r="E53">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>47</v>
+      </c>
+      <c r="C54">
+        <v>48</v>
+      </c>
+      <c r="D54">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>49</v>
+      </c>
+      <c r="C55">
+        <v>55</v>
+      </c>
+      <c r="D55">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>50</v>
+      </c>
+      <c r="C56">
+        <v>54</v>
+      </c>
+      <c r="D56">
+        <v>56</v>
+      </c>
+      <c r="E56">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>50</v>
+      </c>
+      <c r="C57">
+        <v>55</v>
+      </c>
+      <c r="D57">
+        <v>57</v>
+      </c>
+      <c r="E57">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>51</v>
+      </c>
+      <c r="C58">
+        <v>56</v>
+      </c>
+      <c r="D58">
+        <v>58</v>
+      </c>
+      <c r="E58">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>51</v>
+      </c>
+      <c r="C59">
+        <v>57</v>
+      </c>
+      <c r="D59">
+        <v>59</v>
+      </c>
+      <c r="E59">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>52</v>
+      </c>
+      <c r="C60">
+        <v>58</v>
+      </c>
+      <c r="D60">
+        <v>60</v>
+      </c>
+      <c r="E60">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>52</v>
+      </c>
+      <c r="C61">
+        <v>59</v>
+      </c>
+      <c r="D61">
+        <v>61</v>
+      </c>
+      <c r="E61">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>53</v>
+      </c>
+      <c r="C62">
+        <v>60</v>
+      </c>
+      <c r="D62">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>54</v>
+      </c>
+      <c r="C63">
+        <v>55</v>
+      </c>
+      <c r="D63">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>56</v>
+      </c>
+      <c r="C64">
+        <v>57</v>
+      </c>
+      <c r="D64">
+        <v>67</v>
+      </c>
+      <c r="E64">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>58</v>
+      </c>
+      <c r="C65">
+        <v>59</v>
+      </c>
+      <c r="D65">
+        <v>69</v>
+      </c>
+      <c r="E65">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>60</v>
+      </c>
+      <c r="C66">
+        <v>61</v>
+      </c>
+      <c r="D66">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>62</v>
+      </c>
+      <c r="C67">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>63</v>
+      </c>
+      <c r="C68">
+        <v>66</v>
+      </c>
+      <c r="D68">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>63</v>
+      </c>
+      <c r="C69">
+        <v>67</v>
+      </c>
+      <c r="D69">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>64</v>
+      </c>
+      <c r="C70">
+        <v>68</v>
+      </c>
+      <c r="D70">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>64</v>
+      </c>
+      <c r="C71">
+        <v>69</v>
+      </c>
+      <c r="D71">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>65</v>
+      </c>
+      <c r="C72">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDD76D6-043D-4F45-91C3-033B26481F2C}">
+  <dimension ref="A1:D54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>3</v>
+      </c>
+      <c r="C1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>21</v>
+      </c>
+      <c r="D17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>22</v>
+      </c>
+      <c r="D18">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>23</v>
+      </c>
+      <c r="D19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>24</v>
+      </c>
+      <c r="D20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>15</v>
+      </c>
+      <c r="C21">
+        <v>25</v>
+      </c>
+      <c r="D21">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>17</v>
+      </c>
+      <c r="D23">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>17</v>
+      </c>
+      <c r="C24">
+        <v>18</v>
+      </c>
+      <c r="D24">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>19</v>
+      </c>
+      <c r="D25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>19</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>21</v>
+      </c>
+      <c r="C28">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>22</v>
+      </c>
+      <c r="C29">
+        <v>33</v>
+      </c>
+      <c r="D29">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>23</v>
+      </c>
+      <c r="C30">
+        <v>34</v>
+      </c>
+      <c r="D30">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>24</v>
+      </c>
+      <c r="C31">
+        <v>35</v>
+      </c>
+      <c r="D31">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>25</v>
+      </c>
+      <c r="C32">
+        <v>36</v>
+      </c>
+      <c r="D32">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>26</v>
+      </c>
+      <c r="C33">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>27</v>
+      </c>
+      <c r="C34">
+        <v>28</v>
+      </c>
+      <c r="D34">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>28</v>
+      </c>
+      <c r="C35">
+        <v>29</v>
+      </c>
+      <c r="D35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>29</v>
+      </c>
+      <c r="C36">
+        <v>30</v>
+      </c>
+      <c r="D36">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>30</v>
+      </c>
+      <c r="C37">
+        <v>31</v>
+      </c>
+      <c r="D37">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>31</v>
+      </c>
+      <c r="C38">
+        <v>32</v>
+      </c>
+      <c r="D38">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>33</v>
+      </c>
+      <c r="C39">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>34</v>
+      </c>
+      <c r="C40">
+        <v>43</v>
+      </c>
+      <c r="D40">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>35</v>
+      </c>
+      <c r="C41">
+        <v>44</v>
+      </c>
+      <c r="D41">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>36</v>
+      </c>
+      <c r="C42">
+        <v>45</v>
+      </c>
+      <c r="D42">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>37</v>
+      </c>
+      <c r="C43">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>38</v>
+      </c>
+      <c r="C44">
+        <v>39</v>
+      </c>
+      <c r="D44">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>39</v>
+      </c>
+      <c r="C45">
+        <v>40</v>
+      </c>
+      <c r="D45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>40</v>
+      </c>
+      <c r="C46">
+        <v>41</v>
+      </c>
+      <c r="D46">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>41</v>
+      </c>
+      <c r="C47">
+        <v>42</v>
+      </c>
+      <c r="D47">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>43</v>
+      </c>
+      <c r="C48">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>44</v>
+      </c>
+      <c r="C49">
+        <v>51</v>
+      </c>
+      <c r="D49">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>45</v>
+      </c>
+      <c r="C50">
+        <v>52</v>
+      </c>
+      <c r="D50">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>46</v>
+      </c>
+      <c r="C51">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>47</v>
+      </c>
+      <c r="C52">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>48</v>
+      </c>
+      <c r="C53">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>49</v>
+      </c>
+      <c r="C54">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>